<commit_message>
updated output: 10 pages
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="459">
   <si>
     <t>kode_registrasi</t>
   </si>
@@ -103,12 +103,240 @@
     <t>GKL1033521944A1</t>
   </si>
   <si>
+    <t>DKL1333528843A1</t>
+  </si>
+  <si>
+    <t>GKL1833543343A1</t>
+  </si>
+  <si>
+    <t>DKL1202346409A1</t>
+  </si>
+  <si>
+    <t>DKI2365900143A1</t>
+  </si>
+  <si>
+    <t>GKL0433512410A1</t>
+  </si>
+  <si>
+    <t>GKL1102343417A1</t>
+  </si>
+  <si>
+    <t>DKL1102343517A1</t>
+  </si>
+  <si>
+    <t>GKL1522723610B1</t>
+  </si>
+  <si>
+    <t>DKL0922720709A1</t>
+  </si>
+  <si>
+    <t>GKL1140800809A1</t>
+  </si>
+  <si>
+    <t>DKL1140800709A1</t>
+  </si>
+  <si>
+    <t>DKL0819614401A1</t>
+  </si>
+  <si>
+    <t>DTL1920941501A1</t>
+  </si>
+  <si>
+    <t>DBL1111641033A1</t>
+  </si>
+  <si>
+    <t>GKL2408521710A1</t>
+  </si>
+  <si>
+    <t>GKL0308508909A1</t>
+  </si>
+  <si>
+    <t>GBL1825904804A2</t>
+  </si>
+  <si>
+    <t>DKL8525901304A1</t>
+  </si>
+  <si>
+    <t>GKL7225903704A1</t>
+  </si>
+  <si>
+    <t>DKL1625904410A1</t>
+  </si>
+  <si>
+    <t>DTL9021903210B1</t>
+  </si>
+  <si>
+    <t>DTL2021908417A1</t>
+  </si>
+  <si>
+    <t>GTL1818907910A1</t>
+  </si>
+  <si>
+    <t>DTL1818907810A1</t>
+  </si>
+  <si>
+    <t>DKL0234001201A1</t>
+  </si>
+  <si>
+    <t>DKL9822223944A1</t>
+  </si>
+  <si>
+    <t>DBL0022231409A1</t>
+  </si>
+  <si>
+    <t>GKL2302508317A1</t>
+  </si>
+  <si>
+    <t>DKL2302508217A1</t>
+  </si>
+  <si>
+    <t>GKL1705055117A1</t>
+  </si>
+  <si>
+    <t>GKL1705055117B1</t>
+  </si>
+  <si>
+    <t>GKL1705055117C1</t>
+  </si>
+  <si>
+    <t>GKL1933215433A1</t>
+  </si>
+  <si>
+    <t>DKI2360600202A1</t>
+  </si>
+  <si>
+    <t>GKL9819920415A1</t>
+  </si>
+  <si>
+    <t>GBL9819920623A1</t>
+  </si>
+  <si>
+    <t>DKL0427912329A1</t>
+  </si>
+  <si>
+    <t>DTL0933210510A1</t>
+  </si>
+  <si>
+    <t>DKL2405068368A1</t>
+  </si>
+  <si>
+    <t>GTL0305034817A1</t>
+  </si>
+  <si>
+    <t>DBL7605004633B1</t>
+  </si>
+  <si>
+    <t>DKL9405013733A1</t>
+  </si>
+  <si>
+    <t>DBL0305033317A1</t>
+  </si>
+  <si>
+    <t>DTL1831410010A1</t>
+  </si>
+  <si>
+    <t>GKL2415635763A1</t>
+  </si>
+  <si>
+    <t>DKL0816702033B1</t>
+  </si>
+  <si>
+    <t>GKL1505051115B1</t>
+  </si>
+  <si>
+    <t>DKL7200914829A1</t>
+  </si>
+  <si>
+    <t>DBL9117801110A1</t>
+  </si>
+  <si>
+    <t>GKL1707921604B1</t>
+  </si>
+  <si>
+    <t>DKL9807912510B1</t>
+  </si>
+  <si>
+    <t>DKL9807912510A1</t>
+  </si>
+  <si>
+    <t>DKL0213311117B1</t>
+  </si>
+  <si>
+    <t>DKL0413312510A2</t>
+  </si>
+  <si>
+    <t>DKL0413312510B2</t>
+  </si>
+  <si>
+    <t>DBL9610701109A1</t>
+  </si>
+  <si>
+    <t>DTL2406322428A1</t>
+  </si>
+  <si>
+    <t>DTL1406416281A1</t>
+  </si>
+  <si>
+    <t>DKL1706418537A1</t>
+  </si>
+  <si>
+    <t>DTL9613701717A1</t>
+  </si>
+  <si>
+    <t>DTL2022259301A1</t>
+  </si>
+  <si>
+    <t>DKL0928204444A1</t>
+  </si>
+  <si>
+    <t>GKL1436704404A1</t>
+  </si>
+  <si>
+    <t>DKL9304209210A1</t>
+  </si>
+  <si>
+    <t>DPL0433307110B1</t>
+  </si>
+  <si>
+    <t>GKL0133303804A1</t>
+  </si>
+  <si>
+    <t>GKL1833315643A1</t>
+  </si>
+  <si>
+    <t>DKL0333305010A1</t>
+  </si>
+  <si>
+    <t>DKL9933301710A1</t>
+  </si>
+  <si>
+    <t>DKL0433305010B1</t>
+  </si>
+  <si>
+    <t>DKL1240801717A1</t>
+  </si>
+  <si>
+    <t>GKL2022728001A1</t>
+  </si>
+  <si>
+    <t>DKL9002315107A1</t>
+  </si>
+  <si>
+    <t>DKI2468000201A1</t>
+  </si>
+  <si>
     <t>30-09-2024</t>
   </si>
   <si>
     <t>26-09-2024</t>
   </si>
   <si>
+    <t>24-09-2024</t>
+  </si>
+  <si>
+    <t>20-09-2024</t>
+  </si>
+  <si>
     <t>30-09-2029</t>
   </si>
   <si>
@@ -130,6 +358,138 @@
     <t>09-06-2027</t>
   </si>
   <si>
+    <t>26-08-2025</t>
+  </si>
+  <si>
+    <t>02-06-2025</t>
+  </si>
+  <si>
+    <t>02-01-2029</t>
+  </si>
+  <si>
+    <t>24-01-2029</t>
+  </si>
+  <si>
+    <t>24-09-2029</t>
+  </si>
+  <si>
+    <t>17-09-2029</t>
+  </si>
+  <si>
+    <t>23-08-2029</t>
+  </si>
+  <si>
+    <t>12-11-2028</t>
+  </si>
+  <si>
+    <t>28-12-2027</t>
+  </si>
+  <si>
+    <t>26-03-2028</t>
+  </si>
+  <si>
+    <t>16-09-2025</t>
+  </si>
+  <si>
+    <t>23-08-2025</t>
+  </si>
+  <si>
+    <t>20-03-2029</t>
+  </si>
+  <si>
+    <t>25-03-2029</t>
+  </si>
+  <si>
+    <t>07-05-2029</t>
+  </si>
+  <si>
+    <t>03-11-2028</t>
+  </si>
+  <si>
+    <t>16-08-2029</t>
+  </si>
+  <si>
+    <t>08-09-2029</t>
+  </si>
+  <si>
+    <t>16-09-2029</t>
+  </si>
+  <si>
+    <t>09-04-2029</t>
+  </si>
+  <si>
+    <t>10-08-2027</t>
+  </si>
+  <si>
+    <t>23-05-2029</t>
+  </si>
+  <si>
+    <t>06-05-2029</t>
+  </si>
+  <si>
+    <t>11-05-2029</t>
+  </si>
+  <si>
+    <t>20-09-2029</t>
+  </si>
+  <si>
+    <t>11-03-2025</t>
+  </si>
+  <si>
+    <t>22-07-2027</t>
+  </si>
+  <si>
+    <t>08-11-2028</t>
+  </si>
+  <si>
+    <t>21-03-2029</t>
+  </si>
+  <si>
+    <t>07-03-2028</t>
+  </si>
+  <si>
+    <t>02-08-2028</t>
+  </si>
+  <si>
+    <t>29-03-2029</t>
+  </si>
+  <si>
+    <t>27-06-2029</t>
+  </si>
+  <si>
+    <t>08-04-2028</t>
+  </si>
+  <si>
+    <t>23-04-2029</t>
+  </si>
+  <si>
+    <t>04-06-2029</t>
+  </si>
+  <si>
+    <t>01-06-2026</t>
+  </si>
+  <si>
+    <t>21-11-2027</t>
+  </si>
+  <si>
+    <t>23-01-2028</t>
+  </si>
+  <si>
+    <t>28-08-2028</t>
+  </si>
+  <si>
+    <t>31-12-2028</t>
+  </si>
+  <si>
+    <t>19-11-2028</t>
+  </si>
+  <si>
+    <t>31-08-2028</t>
+  </si>
+  <si>
+    <t>27-09-2025</t>
+  </si>
+  <si>
     <t>Direktorat Registrasi Obat</t>
   </si>
   <si>
@@ -175,6 +535,213 @@
     <t>CEFEPIME</t>
   </si>
   <si>
+    <t>DIALIFER</t>
+  </si>
+  <si>
+    <t>IRON SUCROSE</t>
+  </si>
+  <si>
+    <t>CLOVIAR</t>
+  </si>
+  <si>
+    <t>PRIMACAINE 1:100.000</t>
+  </si>
+  <si>
+    <t>LORATADINE</t>
+  </si>
+  <si>
+    <t>DOMPERIDONE MALEATE</t>
+  </si>
+  <si>
+    <t>NOMESIS</t>
+  </si>
+  <si>
+    <t>KALIPAR</t>
+  </si>
+  <si>
+    <t>VALACICLOVIR HCL DIHYDRATE</t>
+  </si>
+  <si>
+    <t>INLACYL</t>
+  </si>
+  <si>
+    <t>RECUSTEIN 300</t>
+  </si>
+  <si>
+    <t>INCETYL</t>
+  </si>
+  <si>
+    <t>PROMAG</t>
+  </si>
+  <si>
+    <t>CARVEDILOL</t>
+  </si>
+  <si>
+    <t>PIRACETAM</t>
+  </si>
+  <si>
+    <t>PARACETAMOL</t>
+  </si>
+  <si>
+    <t>TRIMALGIN</t>
+  </si>
+  <si>
+    <t>METAMIZOLE SODIUM</t>
+  </si>
+  <si>
+    <t>KEMTOV 480</t>
+  </si>
+  <si>
+    <t>MASFLU</t>
+  </si>
+  <si>
+    <t>CORIZINE</t>
+  </si>
+  <si>
+    <t>CETIRIZINE HYDROCHLORIDE</t>
+  </si>
+  <si>
+    <t>CETIRIPIM</t>
+  </si>
+  <si>
+    <t>NOVACYCLINE</t>
+  </si>
+  <si>
+    <t>BIFOTIK</t>
+  </si>
+  <si>
+    <t>POLDAN MIG</t>
+  </si>
+  <si>
+    <t>ETORICOXIB</t>
+  </si>
+  <si>
+    <t>ECOROXIB 120</t>
+  </si>
+  <si>
+    <t>SUCRALFATE</t>
+  </si>
+  <si>
+    <t>GOFEX</t>
+  </si>
+  <si>
+    <t>DICLOFENAC SODIUM</t>
+  </si>
+  <si>
+    <t>ORALIT 200</t>
+  </si>
+  <si>
+    <t>ZENSODERM</t>
+  </si>
+  <si>
+    <t>BROMEDCYL</t>
+  </si>
+  <si>
+    <t>SEVODEX</t>
+  </si>
+  <si>
+    <t>CETIRIZINE HCL</t>
+  </si>
+  <si>
+    <t>DEXANTA</t>
+  </si>
+  <si>
+    <t>VOMETA</t>
+  </si>
+  <si>
+    <t>NEURODEX</t>
+  </si>
+  <si>
+    <t>LOZENTRIN</t>
+  </si>
+  <si>
+    <t>ALBENDAZOLE</t>
+  </si>
+  <si>
+    <t>ORAPROFEN FORTE</t>
+  </si>
+  <si>
+    <t>PANTOPRAZOLE SODIUM SESQUIHYDRATE</t>
+  </si>
+  <si>
+    <t>BUFACORT - N</t>
+  </si>
+  <si>
+    <t>NASPRO</t>
+  </si>
+  <si>
+    <t>DEXAMETHASONE</t>
+  </si>
+  <si>
+    <t>DECASURIK</t>
+  </si>
+  <si>
+    <t>CRAVOX 500</t>
+  </si>
+  <si>
+    <t>MOVIX-7.5</t>
+  </si>
+  <si>
+    <t>MOVIX-15</t>
+  </si>
+  <si>
+    <t>NEUROTROPIC</t>
+  </si>
+  <si>
+    <t>ERLAPAIN</t>
+  </si>
+  <si>
+    <t>ZIPHA</t>
+  </si>
+  <si>
+    <t>ONDASTE</t>
+  </si>
+  <si>
+    <t>BETARHIN</t>
+  </si>
+  <si>
+    <t>ACETIN 200</t>
+  </si>
+  <si>
+    <t>CEFTAMAX</t>
+  </si>
+  <si>
+    <t>ALLOPURINOL 300</t>
+  </si>
+  <si>
+    <t>ULCRON</t>
+  </si>
+  <si>
+    <t>LEXZEPAM 3</t>
+  </si>
+  <si>
+    <t>AMOXICILLIN TRIHYDRATE</t>
+  </si>
+  <si>
+    <t>RANITIDINE HCL</t>
+  </si>
+  <si>
+    <t>SINORIC 100</t>
+  </si>
+  <si>
+    <t>HEXYMER 2</t>
+  </si>
+  <si>
+    <t>SINORIC 300</t>
+  </si>
+  <si>
+    <t>VOMIPER</t>
+  </si>
+  <si>
+    <t>GABAPENTIN</t>
+  </si>
+  <si>
+    <t>SULCOLON</t>
+  </si>
+  <si>
+    <t>BRUKINSA</t>
+  </si>
+  <si>
     <t>INJEKSI; AD 20 ML</t>
   </si>
   <si>
@@ -235,6 +802,183 @@
     <t>SERBUK INJEKSI; 2,024 G</t>
   </si>
   <si>
+    <t>INJEKSI; 400 MG</t>
+  </si>
+  <si>
+    <t>KAPLET SALUT SELAPUT; 612 MG</t>
+  </si>
+  <si>
+    <t>INJEKSI; 40 Mg /18,2 Mcg</t>
+  </si>
+  <si>
+    <t>TABLET; 10,000 MG</t>
+  </si>
+  <si>
+    <t>TABLET SALUT SELAPUT;</t>
+  </si>
+  <si>
+    <t>TABLET; 13,9 MG</t>
+  </si>
+  <si>
+    <t>KAPLET SALUT SELAPUT; 300 MG</t>
+  </si>
+  <si>
+    <t>KAPSUL; 300 MG</t>
+  </si>
+  <si>
+    <t>KAPSUL; 200 MG</t>
+  </si>
+  <si>
+    <t>SUSPENSI; 400 MG /300 MG /100 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 6,25 Mg</t>
+  </si>
+  <si>
+    <t>KAPLET SALUT SELAPUT; 800 MG</t>
+  </si>
+  <si>
+    <t>KAPLET; 500 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 400 MG /80 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 500 MG /2 MG /12,5 MG</t>
+  </si>
+  <si>
+    <t>TABLET SALUT SELAPUT; 10 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 10 MG</t>
+  </si>
+  <si>
+    <t>SERBUK INJEKSI;</t>
+  </si>
+  <si>
+    <t>KAPLET; 400 MG /250 MG /65 MG</t>
+  </si>
+  <si>
+    <t>TABLET SALUT SELAPUT; 120,00 Mg</t>
+  </si>
+  <si>
+    <t>TABLET SALUT SELAPUT; 60 MG</t>
+  </si>
+  <si>
+    <t>TABLET SALUT SELAPUT; 90 MG</t>
+  </si>
+  <si>
+    <t>TABLET SALUT SELAPUT; 120 MG</t>
+  </si>
+  <si>
+    <t>SUSPENSI; 500 MG</t>
+  </si>
+  <si>
+    <t>KAPSUL LUNAK; 400 MG</t>
+  </si>
+  <si>
+    <t>TABLET SALUT ENTERIK; 25 MG</t>
+  </si>
+  <si>
+    <t>SERBUK; 0,300 G /2,700 G /0,580 G /0,520 G</t>
+  </si>
+  <si>
+    <t>SERBUK; 0,300 G /2,700 G /0,520 MG /0,580 G</t>
+  </si>
+  <si>
+    <t>SERBUK; 0,300 G /2,700 G /0,520 G /0,580 G</t>
+  </si>
+  <si>
+    <t>KRIM; 1,2 MG /1,2 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 8,00 MG</t>
+  </si>
+  <si>
+    <t>CAIRAN INHALASI; 250 ML</t>
+  </si>
+  <si>
+    <t>SUSPENSI; 250 MG /644.84 MG /50 MG</t>
+  </si>
+  <si>
+    <t>SUSPENSI; 5 MG</t>
+  </si>
+  <si>
+    <t>TABLET SALUT SELAPUT; 100 MG /200 MG /200 MCG</t>
+  </si>
+  <si>
+    <t>KAPLET KUNYAH; 400,00 MG</t>
+  </si>
+  <si>
+    <t>SUSPENSI; 200 Mg</t>
+  </si>
+  <si>
+    <t>TABLET SALUT ENTERIK; 45,1 Mg</t>
+  </si>
+  <si>
+    <t>KRIM; 5 MG /10 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 300 MG</t>
+  </si>
+  <si>
+    <t>KAPLET; 0,75 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 100 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 7.5 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 15 MG</t>
+  </si>
+  <si>
+    <t>KAPLET SALUT SELAPUT; 100 MG /200 MG /200 Mg</t>
+  </si>
+  <si>
+    <t>GEL; 5 MG</t>
+  </si>
+  <si>
+    <t>TABLET DISPERSIBLE; 54,90 MG</t>
+  </si>
+  <si>
+    <t>SIRUP; 5 MG</t>
+  </si>
+  <si>
+    <t>TABLET SALUT SELAPUT; 10 Mg</t>
+  </si>
+  <si>
+    <t>SERBUK INJEKSI; 1.375 G</t>
+  </si>
+  <si>
+    <t>KAPLET; 300 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 500 MG</t>
+  </si>
+  <si>
+    <t>TABLET; 3.00 MG</t>
+  </si>
+  <si>
+    <t>KAPLET; 573,96 MG</t>
+  </si>
+  <si>
+    <t>INJEKSI; - MG</t>
+  </si>
+  <si>
+    <t>TABLET; 2 MG</t>
+  </si>
+  <si>
+    <t>KAPSUL; 100 MG</t>
+  </si>
+  <si>
+    <t>KAPLET SALUT ENTERIK; 500 MG</t>
+  </si>
+  <si>
+    <t>KAPSUL; 80 MG</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -289,6 +1033,174 @@
     <t>DUS, 1 VIAL @ 1 G</t>
   </si>
   <si>
+    <t>DUS, 5 AMPUL @ 5 ML</t>
+  </si>
+  <si>
+    <t>DUS, 3 BLISTER @ 10 KAPLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 50 CARTRIDGE @ 1,7 ML</t>
+  </si>
+  <si>
+    <t>DUS, 5 STRIP @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 30 BLISTER @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 5 STRIP @ 10 KAPLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 2 STRIP @ 10 KAPSUL</t>
+  </si>
+  <si>
+    <t>DUS, 10 AMPLOP @ 1 STRIP @ 10 KAPSUL</t>
+  </si>
+  <si>
+    <t>DUS, 6 SACHET @ 10 ML</t>
+  </si>
+  <si>
+    <t>DUS, 10 STRIP @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 10 STRIP @ 10 KAPLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 10 AMPLOP @ 1 STRIP @ 10 KAPLET</t>
+  </si>
+  <si>
+    <t>DUS, 10 STRIP @ 10 KAPLET</t>
+  </si>
+  <si>
+    <t>BOTOL PLASTIK @ 100 KAPLET</t>
+  </si>
+  <si>
+    <t>DUS, 10 AMPLOP @ 1 STRIP @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS,10 AMPLOP @1 STRIP @10 TABLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 10 STRIP @10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 25 BLISTER @ 20 KAPSUL</t>
+  </si>
+  <si>
+    <t>DUS, 1 VIAL @ 1 G + 1 AMPUL SANBE - API @ 5 ML</t>
+  </si>
+  <si>
+    <t>DUS, 25 CATCH COVER @ 1 STRIP @ 4 KAPLET</t>
+  </si>
+  <si>
+    <t>DUS, 10 STRIP @ 10 TABLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 3 STRIP @ 10 TABLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 1 BOTOL @ 100 ML</t>
+  </si>
+  <si>
+    <t>DUS, 5 CATCHCOVER @ 1 BLISTER @ 10 KAPSUL LUNAK</t>
+  </si>
+  <si>
+    <t>DUS, 1 BLISTER @ 10 KAPSUL LUNAK</t>
+  </si>
+  <si>
+    <t>DUS, 5 STRIP @ 10 TABLET SALUT ENTERIK</t>
+  </si>
+  <si>
+    <t>DUS,100 SACHET @ 4,129 G</t>
+  </si>
+  <si>
+    <t>DUS, 100 SACHET @ 4,129 G</t>
+  </si>
+  <si>
+    <t>DUS, 1 TUBE @ 10 G</t>
+  </si>
+  <si>
+    <t>DUS, 1 BOTOL @ 250 ML</t>
+  </si>
+  <si>
+    <t>DUS, 6 STRIP @ 10 TABLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 1 BOTOL PLASTIK @ 100 ML</t>
+  </si>
+  <si>
+    <t>DUS, 20 STRIP @ 10 TABLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 5 AMPLOP @ 1 STRIP @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS,10 STRIP @10 KAPLET KUNYAH</t>
+  </si>
+  <si>
+    <t>DUS, 3 STRIP @ 10 TABLET SALUT ENTERIK</t>
+  </si>
+  <si>
+    <t>DUS, 1 TUBE @ 5 G</t>
+  </si>
+  <si>
+    <t>DUS, 25 CATCH COVER @ 1 STRIP @ 4 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 20 STRIP @ 10 KAPLET</t>
+  </si>
+  <si>
+    <t>DUS, 1 STRIP @ 10 TABLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 2 STRIP @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 10 AMPLOP @ 1 STRIP @ 10 KAPLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 1 TUBE @ 20 G</t>
+  </si>
+  <si>
+    <t>DUS, 3 AMPLOP @ 1 STRIP @ 10 TABLET DISPERSIBLE</t>
+  </si>
+  <si>
+    <t>DUS, 1 BOTOL PLASTIK @ 60 ML</t>
+  </si>
+  <si>
+    <t>DUS, 2 AMPLOP @ 1 STRIP @ 10 TABLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 5 AMPLOP @ 1 STRIP @ 10 TABLET SALUT SELAPUT</t>
+  </si>
+  <si>
+    <t>DUS, 3 CATCH COVER @ 1 STRIP @ 10 KAPSUL</t>
+  </si>
+  <si>
+    <t>DUS, 5 BLISTER @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 10 AMPUL @ 2 ML</t>
+  </si>
+  <si>
+    <t>DUS, 6 BLISTER @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 10 BLISTER @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 3 BLISTER @ 10 TABLET</t>
+  </si>
+  <si>
+    <t>DUS, 5 BLISTER @ 10 KAPSUL</t>
+  </si>
+  <si>
+    <t>DUS, 10 STRIP @ 10 KAPLET SALUT ENTERIK</t>
+  </si>
+  <si>
+    <t>DUS, 1 BOTOL @ 120 KAPSUL</t>
+  </si>
+  <si>
     <t>BERNOFARM - Indonesia</t>
   </si>
   <si>
@@ -325,6 +1237,105 @@
     <t>NOVELL PHARMACEUTICAL LABORATORIES - Indonesia</t>
   </si>
   <si>
+    <t>VARIA SEKATA PHARMACEUTICAL LABORATORIES - Indonesia</t>
+  </si>
+  <si>
+    <t>TEMPO SCAN PACIFIC Tbk - Indonesia</t>
+  </si>
+  <si>
+    <t>PERTIWI AGUNG - Indonesia</t>
+  </si>
+  <si>
+    <t>INDOFARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>KALBE FARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>HEXPHARM JAYA LABORATORIES - Indonesia</t>
+  </si>
+  <si>
+    <t>TRIMAN - Indonesia</t>
+  </si>
+  <si>
+    <t>SAMCO FARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>PIM PHARMACEUTICALS - Indonesia</t>
+  </si>
+  <si>
+    <t>NOVAPHARIN - Indonesia</t>
+  </si>
+  <si>
+    <t>SANBE FARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>DIPA PHARMALAB INTERSAINS - Indonesia</t>
+  </si>
+  <si>
+    <t>DEXA MEDICA - Indonesia</t>
+  </si>
+  <si>
+    <t>PROMEDRAHARDJO FARMASI INDUSTRI - Indonesia</t>
+  </si>
+  <si>
+    <t>MEGA LIFESCIENCES INDONESIA - Indonesia</t>
+  </si>
+  <si>
+    <t>PHAPROS Tbk - Indonesia</t>
+  </si>
+  <si>
+    <t>PABRIK PHARMASI ZENITH - Indonesia</t>
+  </si>
+  <si>
+    <t>LLOYD PHARMA INDONESIA - Indonesia</t>
+  </si>
+  <si>
+    <t>MEPROFARM - Indonesia</t>
+  </si>
+  <si>
+    <t>MULIA FARMA SUCI - Indonesia</t>
+  </si>
+  <si>
+    <t>BUFA ANEKA - Indonesia</t>
+  </si>
+  <si>
+    <t>NICHOLAS LABORATORIES INDONESIA - Indonesia</t>
+  </si>
+  <si>
+    <t>HARSEN LABORATORIES - Indonesia</t>
+  </si>
+  <si>
+    <t>LAPI LABORATORIES - Indonesia</t>
+  </si>
+  <si>
+    <t>GLOBAL MULTI PHARMALAB - Indonesia</t>
+  </si>
+  <si>
+    <t>ERLANGGA EDI LABORATORIES (ERELA) - Indonesia</t>
+  </si>
+  <si>
+    <t>ERLIMPEX - Indonesia</t>
+  </si>
+  <si>
+    <t>MAHAKAM BETA FARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>SIMEX PHARMACEUTICAL INDONESIA - Indonesia</t>
+  </si>
+  <si>
+    <t>SEJAHTERA LESTARI FARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>CORONET CROWN - Indonesia</t>
+  </si>
+  <si>
+    <t>MERSIFARMA TIRMAKU MERCUSANA - Indonesia</t>
+  </si>
+  <si>
+    <t>ETANA BIOTECHNOLOGIES INDONESIA - Indonesia</t>
+  </si>
+  <si>
     <t>ASTRAZENECA AB - Sweden</t>
   </si>
   <si>
@@ -341,6 +1352,45 @@
   </si>
   <si>
     <t>ETERCON PHARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>LABORATORIOS INIBSA, S.A. - Spain</t>
+  </si>
+  <si>
+    <t>BINTANG TOEDJOE - Indonesia</t>
+  </si>
+  <si>
+    <t>DANKOS FARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>SANBE FARMA (UNIT 2) - Indonesia</t>
+  </si>
+  <si>
+    <t>CAPRIFARMINDO LABORATORIES - Indonesia</t>
+  </si>
+  <si>
+    <t>MEGA LIFESCIENCES PUBLIC COMPANY LIMITED - Thailand</t>
+  </si>
+  <si>
+    <t>LUCAS DJAJA - Indonesia</t>
+  </si>
+  <si>
+    <t>KIMIA FARMA TBK - Indonesia</t>
+  </si>
+  <si>
+    <t>FERRON PAR PHARMACEUTICALS - Indonesia</t>
+  </si>
+  <si>
+    <t>BETA PHARMACON - Indonesia</t>
+  </si>
+  <si>
+    <t>MUTIARA MUKTI FARMA - Indonesia</t>
+  </si>
+  <si>
+    <t>SANBE FARMA (UNIT 1) - Indonesia</t>
+  </si>
+  <si>
+    <t>CATALENT CTS, LLC - United States of America</t>
   </si>
 </sst>
 </file>
@@ -698,7 +1748,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -708,11 +1758,11 @@
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="46.7109375" customWidth="1"/>
-    <col min="9" max="9" width="51.7109375" customWidth="1"/>
+    <col min="8" max="8" width="55.7109375" customWidth="1"/>
+    <col min="9" max="9" width="57.7109375" customWidth="1"/>
     <col min="10" max="10" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -753,31 +1803,31 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>242</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>322</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -785,31 +1835,31 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>323</v>
       </c>
       <c r="I3" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
       <c r="J3" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -817,31 +1867,31 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>244</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>324</v>
       </c>
       <c r="I4" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
       <c r="J4" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -849,31 +1899,31 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>245</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>325</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
       <c r="J5" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -881,31 +1931,31 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>160</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>246</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>326</v>
       </c>
       <c r="I6" t="s">
-        <v>92</v>
+        <v>396</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -913,31 +1963,31 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>247</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>327</v>
       </c>
       <c r="I7" t="s">
-        <v>93</v>
+        <v>397</v>
       </c>
       <c r="J7" t="s">
-        <v>104</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -945,31 +1995,31 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>248</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>328</v>
       </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>397</v>
       </c>
       <c r="J8" t="s">
-        <v>105</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -977,31 +2027,31 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>249</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>329</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>398</v>
       </c>
       <c r="J9" t="s">
-        <v>94</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1009,31 +2059,31 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>250</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
+        <v>330</v>
       </c>
       <c r="I10" t="s">
-        <v>94</v>
+        <v>398</v>
       </c>
       <c r="J10" t="s">
-        <v>94</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1041,31 +2091,31 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>164</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>251</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>331</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>398</v>
       </c>
       <c r="J11" t="s">
-        <v>94</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1073,31 +2123,31 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>252</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>332</v>
       </c>
       <c r="I12" t="s">
-        <v>95</v>
+        <v>399</v>
       </c>
       <c r="J12" t="s">
-        <v>95</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1105,31 +2155,31 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
+        <v>333</v>
       </c>
       <c r="I13" t="s">
-        <v>96</v>
+        <v>400</v>
       </c>
       <c r="J13" t="s">
-        <v>96</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1137,31 +2187,31 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>167</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>254</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>334</v>
       </c>
       <c r="I14" t="s">
-        <v>97</v>
+        <v>401</v>
       </c>
       <c r="J14" t="s">
-        <v>106</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1169,31 +2219,31 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>167</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>255</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
+        <v>334</v>
       </c>
       <c r="I15" t="s">
-        <v>97</v>
+        <v>401</v>
       </c>
       <c r="J15" t="s">
-        <v>106</v>
+        <v>443</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1201,31 +2251,31 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>168</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>256</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>323</v>
       </c>
       <c r="I16" t="s">
-        <v>98</v>
+        <v>402</v>
       </c>
       <c r="J16" t="s">
-        <v>98</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1233,31 +2283,31 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>257</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H17" t="s">
-        <v>87</v>
+        <v>335</v>
       </c>
       <c r="I17" t="s">
-        <v>99</v>
+        <v>403</v>
       </c>
       <c r="J17" t="s">
-        <v>107</v>
+        <v>444</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1265,31 +2315,31 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>258</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H18" t="s">
-        <v>87</v>
+        <v>335</v>
       </c>
       <c r="I18" t="s">
-        <v>99</v>
+        <v>403</v>
       </c>
       <c r="J18" t="s">
-        <v>107</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1297,31 +2347,31 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>259</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H19" t="s">
-        <v>88</v>
+        <v>336</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>404</v>
       </c>
       <c r="J19" t="s">
-        <v>91</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1329,31 +2379,31 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>171</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>260</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>321</v>
       </c>
       <c r="H20" t="s">
-        <v>89</v>
+        <v>337</v>
       </c>
       <c r="I20" t="s">
-        <v>101</v>
+        <v>405</v>
       </c>
       <c r="J20" t="s">
-        <v>101</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1361,31 +2411,2591 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" t="s">
+        <v>261</v>
+      </c>
+      <c r="G21" t="s">
+        <v>321</v>
+      </c>
+      <c r="H21" t="s">
+        <v>338</v>
+      </c>
+      <c r="I21" t="s">
+        <v>406</v>
+      </c>
+      <c r="J21" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F22" t="s">
+        <v>262</v>
+      </c>
+      <c r="G22" t="s">
+        <v>321</v>
+      </c>
+      <c r="H22" t="s">
+        <v>339</v>
+      </c>
+      <c r="I22" t="s">
+        <v>406</v>
+      </c>
+      <c r="J22" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" t="s">
+        <v>262</v>
+      </c>
+      <c r="G23" t="s">
+        <v>321</v>
+      </c>
+      <c r="H23" t="s">
+        <v>339</v>
+      </c>
+      <c r="I23" t="s">
+        <v>406</v>
+      </c>
+      <c r="J23" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G24" t="s">
+        <v>321</v>
+      </c>
+      <c r="H24" t="s">
+        <v>340</v>
+      </c>
+      <c r="I24" t="s">
+        <v>395</v>
+      </c>
+      <c r="J24" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" t="s">
+        <v>264</v>
+      </c>
+      <c r="G25" t="s">
+        <v>321</v>
+      </c>
+      <c r="H25" t="s">
+        <v>341</v>
+      </c>
+      <c r="I25" t="s">
+        <v>407</v>
+      </c>
+      <c r="J25" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" t="s">
+        <v>265</v>
+      </c>
+      <c r="G26" t="s">
+        <v>321</v>
+      </c>
+      <c r="H26" t="s">
+        <v>342</v>
+      </c>
+      <c r="I26" t="s">
+        <v>406</v>
+      </c>
+      <c r="J26" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" t="s">
+        <v>178</v>
+      </c>
+      <c r="F27" t="s">
+        <v>266</v>
+      </c>
+      <c r="G27" t="s">
+        <v>321</v>
+      </c>
+      <c r="H27" t="s">
+        <v>331</v>
+      </c>
+      <c r="I27" t="s">
+        <v>395</v>
+      </c>
+      <c r="J27" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" t="s">
+        <v>158</v>
+      </c>
+      <c r="E28" t="s">
+        <v>179</v>
+      </c>
+      <c r="F28" t="s">
+        <v>266</v>
+      </c>
+      <c r="G28" t="s">
+        <v>321</v>
+      </c>
+      <c r="H28" t="s">
+        <v>334</v>
+      </c>
+      <c r="I28" t="s">
+        <v>395</v>
+      </c>
+      <c r="J28" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" t="s">
+        <v>169</v>
+      </c>
+      <c r="F29" t="s">
+        <v>267</v>
+      </c>
+      <c r="G29" t="s">
+        <v>321</v>
+      </c>
+      <c r="H29" t="s">
+        <v>343</v>
+      </c>
+      <c r="I29" t="s">
+        <v>408</v>
+      </c>
+      <c r="J29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
         <v>37</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" t="s">
+        <v>158</v>
+      </c>
+      <c r="E30" t="s">
+        <v>180</v>
+      </c>
+      <c r="F30" t="s">
+        <v>268</v>
+      </c>
+      <c r="G30" t="s">
+        <v>321</v>
+      </c>
+      <c r="H30" t="s">
+        <v>344</v>
+      </c>
+      <c r="I30" t="s">
+        <v>408</v>
+      </c>
+      <c r="J30" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="E21" t="s">
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E31" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" t="s">
+        <v>263</v>
+      </c>
+      <c r="G31" t="s">
+        <v>321</v>
+      </c>
+      <c r="H31" t="s">
+        <v>340</v>
+      </c>
+      <c r="I31" t="s">
+        <v>404</v>
+      </c>
+      <c r="J31" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" t="s">
+        <v>182</v>
+      </c>
+      <c r="F32" t="s">
+        <v>263</v>
+      </c>
+      <c r="G32" t="s">
+        <v>321</v>
+      </c>
+      <c r="H32" t="s">
+        <v>340</v>
+      </c>
+      <c r="I32" t="s">
+        <v>404</v>
+      </c>
+      <c r="J32" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" t="s">
+        <v>183</v>
+      </c>
+      <c r="F33" t="s">
+        <v>269</v>
+      </c>
+      <c r="G33" t="s">
+        <v>321</v>
+      </c>
+      <c r="H33" t="s">
+        <v>345</v>
+      </c>
+      <c r="I33" t="s">
+        <v>409</v>
+      </c>
+      <c r="J33" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F34" t="s">
+        <v>270</v>
+      </c>
+      <c r="G34" t="s">
+        <v>321</v>
+      </c>
+      <c r="H34" t="s">
+        <v>346</v>
+      </c>
+      <c r="I34" t="s">
+        <v>410</v>
+      </c>
+      <c r="J34" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" t="s">
+        <v>185</v>
+      </c>
+      <c r="F35" t="s">
+        <v>271</v>
+      </c>
+      <c r="G35" t="s">
+        <v>321</v>
+      </c>
+      <c r="H35" t="s">
+        <v>347</v>
+      </c>
+      <c r="I35" t="s">
+        <v>411</v>
+      </c>
+      <c r="J35" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" t="s">
+        <v>186</v>
+      </c>
+      <c r="F36" t="s">
+        <v>272</v>
+      </c>
+      <c r="G36" t="s">
+        <v>321</v>
+      </c>
+      <c r="H36" t="s">
+        <v>348</v>
+      </c>
+      <c r="I36" t="s">
+        <v>412</v>
+      </c>
+      <c r="J36" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" t="s">
+        <v>187</v>
+      </c>
+      <c r="F37" t="s">
+        <v>273</v>
+      </c>
+      <c r="G37" t="s">
+        <v>321</v>
+      </c>
+      <c r="H37" t="s">
+        <v>349</v>
+      </c>
+      <c r="I37" t="s">
+        <v>412</v>
+      </c>
+      <c r="J37" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" t="s">
+        <v>158</v>
+      </c>
+      <c r="E38" t="s">
+        <v>188</v>
+      </c>
+      <c r="F38" t="s">
+        <v>274</v>
+      </c>
+      <c r="G38" t="s">
+        <v>321</v>
+      </c>
+      <c r="H38" t="s">
+        <v>350</v>
+      </c>
+      <c r="I38" t="s">
+        <v>413</v>
+      </c>
+      <c r="J38" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" t="s">
+        <v>189</v>
+      </c>
+      <c r="F39" t="s">
+        <v>274</v>
+      </c>
+      <c r="G39" t="s">
+        <v>321</v>
+      </c>
+      <c r="H39" t="s">
+        <v>351</v>
+      </c>
+      <c r="I39" t="s">
+        <v>413</v>
+      </c>
+      <c r="J39" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" t="s">
+        <v>190</v>
+      </c>
+      <c r="F40" t="s">
+        <v>274</v>
+      </c>
+      <c r="G40" t="s">
+        <v>321</v>
+      </c>
+      <c r="H40" t="s">
+        <v>352</v>
+      </c>
+      <c r="I40" t="s">
+        <v>413</v>
+      </c>
+      <c r="J40" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" t="s">
+        <v>191</v>
+      </c>
+      <c r="F41" t="s">
+        <v>275</v>
+      </c>
+      <c r="G41" t="s">
+        <v>321</v>
+      </c>
+      <c r="H41" t="s">
+        <v>348</v>
+      </c>
+      <c r="I41" t="s">
+        <v>413</v>
+      </c>
+      <c r="J41" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" t="s">
+        <v>158</v>
+      </c>
+      <c r="E42" t="s">
+        <v>192</v>
+      </c>
+      <c r="F42" t="s">
+        <v>276</v>
+      </c>
+      <c r="G42" t="s">
+        <v>321</v>
+      </c>
+      <c r="H42" t="s">
+        <v>353</v>
+      </c>
+      <c r="I42" t="s">
+        <v>414</v>
+      </c>
+      <c r="J42" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" t="s">
+        <v>158</v>
+      </c>
+      <c r="E43" t="s">
+        <v>193</v>
+      </c>
+      <c r="F43" t="s">
+        <v>277</v>
+      </c>
+      <c r="G43" t="s">
+        <v>321</v>
+      </c>
+      <c r="H43" t="s">
+        <v>354</v>
+      </c>
+      <c r="I43" t="s">
+        <v>414</v>
+      </c>
+      <c r="J43" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" t="s">
+        <v>194</v>
+      </c>
+      <c r="F44" t="s">
+        <v>278</v>
+      </c>
+      <c r="G44" t="s">
+        <v>321</v>
+      </c>
+      <c r="H44" t="s">
+        <v>355</v>
+      </c>
+      <c r="I44" t="s">
+        <v>415</v>
+      </c>
+      <c r="J44" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" t="s">
         <v>52</v>
       </c>
-      <c r="F21" t="s">
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" t="s">
+        <v>158</v>
+      </c>
+      <c r="E45" t="s">
+        <v>195</v>
+      </c>
+      <c r="F45" t="s">
+        <v>278</v>
+      </c>
+      <c r="G45" t="s">
+        <v>321</v>
+      </c>
+      <c r="H45" t="s">
+        <v>348</v>
+      </c>
+      <c r="I45" t="s">
+        <v>415</v>
+      </c>
+      <c r="J45" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" t="s">
+        <v>196</v>
+      </c>
+      <c r="F46" t="s">
+        <v>247</v>
+      </c>
+      <c r="G46" t="s">
+        <v>321</v>
+      </c>
+      <c r="H46" t="s">
+        <v>356</v>
+      </c>
+      <c r="I46" t="s">
+        <v>416</v>
+      </c>
+      <c r="J46" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" t="s">
+        <v>158</v>
+      </c>
+      <c r="E47" t="s">
+        <v>197</v>
+      </c>
+      <c r="F47" t="s">
+        <v>279</v>
+      </c>
+      <c r="G47" t="s">
+        <v>321</v>
+      </c>
+      <c r="H47" t="s">
+        <v>357</v>
+      </c>
+      <c r="I47" t="s">
+        <v>417</v>
+      </c>
+      <c r="J47" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" t="s">
+        <v>198</v>
+      </c>
+      <c r="F48" t="s">
+        <v>280</v>
+      </c>
+      <c r="G48" t="s">
+        <v>321</v>
+      </c>
+      <c r="H48" t="s">
+        <v>358</v>
+      </c>
+      <c r="I48" t="s">
+        <v>417</v>
+      </c>
+      <c r="J48" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" t="s">
+        <v>158</v>
+      </c>
+      <c r="E49" t="s">
+        <v>199</v>
+      </c>
+      <c r="F49" t="s">
+        <v>281</v>
+      </c>
+      <c r="G49" t="s">
+        <v>321</v>
+      </c>
+      <c r="H49" t="s">
+        <v>359</v>
+      </c>
+      <c r="I49" t="s">
+        <v>418</v>
+      </c>
+      <c r="J49" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D50" t="s">
+        <v>158</v>
+      </c>
+      <c r="E50" t="s">
+        <v>200</v>
+      </c>
+      <c r="F50" t="s">
+        <v>281</v>
+      </c>
+      <c r="G50" t="s">
+        <v>321</v>
+      </c>
+      <c r="H50" t="s">
+        <v>360</v>
+      </c>
+      <c r="I50" t="s">
+        <v>418</v>
+      </c>
+      <c r="J50" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" t="s">
+        <v>199</v>
+      </c>
+      <c r="F51" t="s">
+        <v>282</v>
+      </c>
+      <c r="G51" t="s">
+        <v>321</v>
+      </c>
+      <c r="H51" t="s">
+        <v>360</v>
+      </c>
+      <c r="I51" t="s">
+        <v>419</v>
+      </c>
+      <c r="J51" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" t="s">
+        <v>199</v>
+      </c>
+      <c r="F52" t="s">
+        <v>283</v>
+      </c>
+      <c r="G52" t="s">
+        <v>321</v>
+      </c>
+      <c r="H52" t="s">
+        <v>360</v>
+      </c>
+      <c r="I52" t="s">
+        <v>419</v>
+      </c>
+      <c r="J52" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
+        <v>127</v>
+      </c>
+      <c r="D53" t="s">
+        <v>158</v>
+      </c>
+      <c r="E53" t="s">
+        <v>199</v>
+      </c>
+      <c r="F53" t="s">
+        <v>284</v>
+      </c>
+      <c r="G53" t="s">
+        <v>321</v>
+      </c>
+      <c r="H53" t="s">
+        <v>360</v>
+      </c>
+      <c r="I53" t="s">
+        <v>419</v>
+      </c>
+      <c r="J53" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" t="s">
+        <v>158</v>
+      </c>
+      <c r="E54" t="s">
+        <v>201</v>
+      </c>
+      <c r="F54" t="s">
+        <v>285</v>
+      </c>
+      <c r="G54" t="s">
+        <v>321</v>
+      </c>
+      <c r="H54" t="s">
+        <v>361</v>
+      </c>
+      <c r="I54" t="s">
+        <v>420</v>
+      </c>
+      <c r="J54" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" t="s">
+        <v>158</v>
+      </c>
+      <c r="E55" t="s">
+        <v>202</v>
+      </c>
+      <c r="F55" t="s">
+        <v>286</v>
+      </c>
+      <c r="G55" t="s">
+        <v>321</v>
+      </c>
+      <c r="H55" t="s">
+        <v>362</v>
+      </c>
+      <c r="I55" t="s">
+        <v>421</v>
+      </c>
+      <c r="J55" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" t="s">
+        <v>129</v>
+      </c>
+      <c r="D56" t="s">
+        <v>158</v>
+      </c>
+      <c r="E56" t="s">
+        <v>202</v>
+      </c>
+      <c r="F56" t="s">
+        <v>286</v>
+      </c>
+      <c r="G56" t="s">
+        <v>321</v>
+      </c>
+      <c r="H56" t="s">
+        <v>363</v>
+      </c>
+      <c r="I56" t="s">
+        <v>421</v>
+      </c>
+      <c r="J56" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
+      </c>
+      <c r="D57" t="s">
+        <v>158</v>
+      </c>
+      <c r="E57" t="s">
+        <v>203</v>
+      </c>
+      <c r="F57" t="s">
+        <v>287</v>
+      </c>
+      <c r="G57" t="s">
+        <v>321</v>
+      </c>
+      <c r="H57" t="s">
+        <v>364</v>
+      </c>
+      <c r="I57" t="s">
+        <v>422</v>
+      </c>
+      <c r="J57" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" t="s">
+        <v>131</v>
+      </c>
+      <c r="D58" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58" t="s">
+        <v>204</v>
+      </c>
+      <c r="F58" t="s">
+        <v>288</v>
+      </c>
+      <c r="G58" t="s">
+        <v>321</v>
+      </c>
+      <c r="H58" t="s">
+        <v>365</v>
+      </c>
+      <c r="I58" t="s">
+        <v>422</v>
+      </c>
+      <c r="J58" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" t="s">
+        <v>158</v>
+      </c>
+      <c r="E59" t="s">
+        <v>204</v>
+      </c>
+      <c r="F59" t="s">
+        <v>289</v>
+      </c>
+      <c r="G59" t="s">
+        <v>321</v>
+      </c>
+      <c r="H59" t="s">
+        <v>366</v>
+      </c>
+      <c r="I59" t="s">
+        <v>422</v>
+      </c>
+      <c r="J59" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" t="s">
+        <v>158</v>
+      </c>
+      <c r="E60" t="s">
+        <v>204</v>
+      </c>
+      <c r="F60" t="s">
+        <v>290</v>
+      </c>
+      <c r="G60" t="s">
+        <v>321</v>
+      </c>
+      <c r="H60" t="s">
+        <v>366</v>
+      </c>
+      <c r="I60" t="s">
+        <v>422</v>
+      </c>
+      <c r="J60" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" t="s">
+        <v>158</v>
+      </c>
+      <c r="E61" t="s">
+        <v>205</v>
+      </c>
+      <c r="F61" t="s">
+        <v>291</v>
+      </c>
+      <c r="G61" t="s">
+        <v>321</v>
+      </c>
+      <c r="H61" t="s">
+        <v>367</v>
+      </c>
+      <c r="I61" t="s">
+        <v>423</v>
+      </c>
+      <c r="J61" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" t="s">
+        <v>158</v>
+      </c>
+      <c r="E62" t="s">
+        <v>206</v>
+      </c>
+      <c r="F62" t="s">
+        <v>292</v>
+      </c>
+      <c r="G62" t="s">
+        <v>321</v>
+      </c>
+      <c r="H62" t="s">
+        <v>353</v>
+      </c>
+      <c r="I62" t="s">
+        <v>420</v>
+      </c>
+      <c r="J62" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" t="s">
+        <v>134</v>
+      </c>
+      <c r="D63" t="s">
+        <v>158</v>
+      </c>
+      <c r="E63" t="s">
+        <v>207</v>
+      </c>
+      <c r="F63" t="s">
+        <v>293</v>
+      </c>
+      <c r="G63" t="s">
+        <v>321</v>
+      </c>
+      <c r="H63" t="s">
+        <v>368</v>
+      </c>
+      <c r="I63" t="s">
+        <v>419</v>
+      </c>
+      <c r="J63" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" t="s">
+        <v>135</v>
+      </c>
+      <c r="D64" t="s">
+        <v>158</v>
+      </c>
+      <c r="E64" t="s">
+        <v>208</v>
+      </c>
+      <c r="F64" t="s">
+        <v>277</v>
+      </c>
+      <c r="G64" t="s">
+        <v>321</v>
+      </c>
+      <c r="H64" t="s">
+        <v>369</v>
+      </c>
+      <c r="I64" t="s">
+        <v>419</v>
+      </c>
+      <c r="J64" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" t="s">
+        <v>158</v>
+      </c>
+      <c r="E65" t="s">
+        <v>209</v>
+      </c>
+      <c r="F65" t="s">
+        <v>294</v>
+      </c>
+      <c r="G65" t="s">
+        <v>321</v>
+      </c>
+      <c r="H65" t="s">
+        <v>370</v>
+      </c>
+      <c r="I65" t="s">
+        <v>419</v>
+      </c>
+      <c r="J65" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" t="s">
+        <v>158</v>
+      </c>
+      <c r="E66" t="s">
+        <v>210</v>
+      </c>
+      <c r="F66" t="s">
+        <v>295</v>
+      </c>
+      <c r="G66" t="s">
+        <v>321</v>
+      </c>
+      <c r="H66" t="s">
+        <v>336</v>
+      </c>
+      <c r="I66" t="s">
+        <v>419</v>
+      </c>
+      <c r="J66" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67" t="s">
+        <v>158</v>
+      </c>
+      <c r="E67" t="s">
+        <v>211</v>
+      </c>
+      <c r="F67" t="s">
+        <v>296</v>
+      </c>
+      <c r="G67" t="s">
+        <v>321</v>
+      </c>
+      <c r="H67" t="s">
+        <v>371</v>
+      </c>
+      <c r="I67" t="s">
+        <v>419</v>
+      </c>
+      <c r="J67" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" t="s">
         <v>72</v>
       </c>
-      <c r="G21" t="s">
+      <c r="B68" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" t="s">
+        <v>158</v>
+      </c>
+      <c r="E68" t="s">
+        <v>212</v>
+      </c>
+      <c r="F68" t="s">
+        <v>278</v>
+      </c>
+      <c r="G68" t="s">
+        <v>321</v>
+      </c>
+      <c r="H68" t="s">
+        <v>372</v>
+      </c>
+      <c r="I68" t="s">
+        <v>424</v>
+      </c>
+      <c r="J68" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" t="s">
         <v>73</v>
       </c>
-      <c r="H21" t="s">
+      <c r="B69" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" t="s">
+        <v>138</v>
+      </c>
+      <c r="D69" t="s">
+        <v>158</v>
+      </c>
+      <c r="E69" t="s">
+        <v>213</v>
+      </c>
+      <c r="F69" t="s">
+        <v>297</v>
+      </c>
+      <c r="G69" t="s">
+        <v>321</v>
+      </c>
+      <c r="H69" t="s">
+        <v>373</v>
+      </c>
+      <c r="I69" t="s">
+        <v>425</v>
+      </c>
+      <c r="J69" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" t="s">
+        <v>158</v>
+      </c>
+      <c r="E70" t="s">
+        <v>214</v>
+      </c>
+      <c r="F70" t="s">
+        <v>298</v>
+      </c>
+      <c r="G70" t="s">
+        <v>321</v>
+      </c>
+      <c r="H70" t="s">
+        <v>336</v>
+      </c>
+      <c r="I70" t="s">
+        <v>426</v>
+      </c>
+      <c r="J70" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" t="s">
+        <v>158</v>
+      </c>
+      <c r="E71" t="s">
+        <v>215</v>
+      </c>
+      <c r="F71" t="s">
+        <v>299</v>
+      </c>
+      <c r="G71" t="s">
+        <v>321</v>
+      </c>
+      <c r="H71" t="s">
+        <v>374</v>
+      </c>
+      <c r="I71" t="s">
+        <v>419</v>
+      </c>
+      <c r="J71" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" t="s">
+        <v>141</v>
+      </c>
+      <c r="D72" t="s">
+        <v>158</v>
+      </c>
+      <c r="E72" t="s">
+        <v>211</v>
+      </c>
+      <c r="F72" t="s">
+        <v>296</v>
+      </c>
+      <c r="G72" t="s">
+        <v>321</v>
+      </c>
+      <c r="H72" t="s">
+        <v>371</v>
+      </c>
+      <c r="I72" t="s">
+        <v>419</v>
+      </c>
+      <c r="J72" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" t="s">
+        <v>158</v>
+      </c>
+      <c r="E73" t="s">
+        <v>210</v>
+      </c>
+      <c r="F73" t="s">
+        <v>295</v>
+      </c>
+      <c r="G73" t="s">
+        <v>321</v>
+      </c>
+      <c r="H73" t="s">
+        <v>336</v>
+      </c>
+      <c r="I73" t="s">
+        <v>419</v>
+      </c>
+      <c r="J73" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" t="s">
+        <v>158</v>
+      </c>
+      <c r="E74" t="s">
+        <v>216</v>
+      </c>
+      <c r="F74" t="s">
+        <v>300</v>
+      </c>
+      <c r="G74" t="s">
+        <v>321</v>
+      </c>
+      <c r="H74" t="s">
+        <v>375</v>
+      </c>
+      <c r="I74" t="s">
+        <v>427</v>
+      </c>
+      <c r="J74" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" t="s">
+        <v>143</v>
+      </c>
+      <c r="D75" t="s">
+        <v>158</v>
+      </c>
+      <c r="E75" t="s">
+        <v>217</v>
+      </c>
+      <c r="F75" t="s">
+        <v>301</v>
+      </c>
+      <c r="G75" t="s">
+        <v>321</v>
+      </c>
+      <c r="H75" t="s">
+        <v>376</v>
+      </c>
+      <c r="I75" t="s">
+        <v>428</v>
+      </c>
+      <c r="J75" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" t="s">
+        <v>144</v>
+      </c>
+      <c r="D76" t="s">
+        <v>158</v>
+      </c>
+      <c r="E76" t="s">
+        <v>218</v>
+      </c>
+      <c r="F76" t="s">
+        <v>302</v>
+      </c>
+      <c r="G76" t="s">
+        <v>321</v>
+      </c>
+      <c r="H76" t="s">
+        <v>377</v>
+      </c>
+      <c r="I76" t="s">
+        <v>429</v>
+      </c>
+      <c r="J76" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
+        <v>106</v>
+      </c>
+      <c r="C77" t="s">
+        <v>145</v>
+      </c>
+      <c r="D77" t="s">
+        <v>158</v>
+      </c>
+      <c r="E77" t="s">
+        <v>219</v>
+      </c>
+      <c r="F77" t="s">
+        <v>301</v>
+      </c>
+      <c r="G77" t="s">
+        <v>321</v>
+      </c>
+      <c r="H77" t="s">
+        <v>348</v>
+      </c>
+      <c r="I77" t="s">
+        <v>429</v>
+      </c>
+      <c r="J77" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" t="s">
+        <v>106</v>
+      </c>
+      <c r="C78" t="s">
+        <v>145</v>
+      </c>
+      <c r="D78" t="s">
+        <v>158</v>
+      </c>
+      <c r="E78" t="s">
+        <v>219</v>
+      </c>
+      <c r="F78" t="s">
+        <v>303</v>
+      </c>
+      <c r="G78" t="s">
+        <v>321</v>
+      </c>
+      <c r="H78" t="s">
+        <v>348</v>
+      </c>
+      <c r="I78" t="s">
+        <v>429</v>
+      </c>
+      <c r="J78" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" t="s">
+        <v>106</v>
+      </c>
+      <c r="C79" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" t="s">
+        <v>158</v>
+      </c>
+      <c r="E79" t="s">
+        <v>220</v>
+      </c>
+      <c r="F79" t="s">
+        <v>266</v>
+      </c>
+      <c r="G79" t="s">
+        <v>321</v>
+      </c>
+      <c r="H79" t="s">
+        <v>378</v>
+      </c>
+      <c r="I79" t="s">
+        <v>430</v>
+      </c>
+      <c r="J79" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" t="s">
+        <v>106</v>
+      </c>
+      <c r="C80" t="s">
+        <v>115</v>
+      </c>
+      <c r="D80" t="s">
+        <v>158</v>
+      </c>
+      <c r="E80" t="s">
+        <v>221</v>
+      </c>
+      <c r="F80" t="s">
+        <v>304</v>
+      </c>
+      <c r="G80" t="s">
+        <v>321</v>
+      </c>
+      <c r="H80" t="s">
+        <v>379</v>
+      </c>
+      <c r="I80" t="s">
+        <v>430</v>
+      </c>
+      <c r="J80" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" t="s">
+        <v>115</v>
+      </c>
+      <c r="D81" t="s">
+        <v>158</v>
+      </c>
+      <c r="E81" t="s">
+        <v>222</v>
+      </c>
+      <c r="F81" t="s">
+        <v>305</v>
+      </c>
+      <c r="G81" t="s">
+        <v>321</v>
+      </c>
+      <c r="H81" t="s">
+        <v>379</v>
+      </c>
+      <c r="I81" t="s">
+        <v>430</v>
+      </c>
+      <c r="J81" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" t="s">
+        <v>147</v>
+      </c>
+      <c r="D82" t="s">
+        <v>158</v>
+      </c>
+      <c r="E82" t="s">
+        <v>223</v>
+      </c>
+      <c r="F82" t="s">
+        <v>306</v>
+      </c>
+      <c r="G82" t="s">
+        <v>321</v>
+      </c>
+      <c r="H82" t="s">
+        <v>380</v>
+      </c>
+      <c r="I82" t="s">
+        <v>431</v>
+      </c>
+      <c r="J82" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" t="s">
+        <v>106</v>
+      </c>
+      <c r="C83" t="s">
+        <v>148</v>
+      </c>
+      <c r="D83" t="s">
+        <v>158</v>
+      </c>
+      <c r="E83" t="s">
+        <v>224</v>
+      </c>
+      <c r="F83" t="s">
+        <v>307</v>
+      </c>
+      <c r="G83" t="s">
+        <v>321</v>
+      </c>
+      <c r="H83" t="s">
+        <v>381</v>
+      </c>
+      <c r="I83" t="s">
+        <v>432</v>
+      </c>
+      <c r="J83" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" t="s">
+        <v>149</v>
+      </c>
+      <c r="D84" t="s">
+        <v>158</v>
+      </c>
+      <c r="E84" t="s">
+        <v>225</v>
+      </c>
+      <c r="F84" t="s">
+        <v>308</v>
+      </c>
+      <c r="G84" t="s">
+        <v>321</v>
+      </c>
+      <c r="H84" t="s">
+        <v>382</v>
+      </c>
+      <c r="I84" t="s">
+        <v>433</v>
+      </c>
+      <c r="J84" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" t="s">
+        <v>106</v>
+      </c>
+      <c r="C85" t="s">
+        <v>120</v>
+      </c>
+      <c r="D85" t="s">
+        <v>158</v>
+      </c>
+      <c r="E85" t="s">
+        <v>226</v>
+      </c>
+      <c r="F85" t="s">
+        <v>309</v>
+      </c>
+      <c r="G85" t="s">
+        <v>321</v>
+      </c>
+      <c r="H85" t="s">
+        <v>383</v>
+      </c>
+      <c r="I85" t="s">
+        <v>433</v>
+      </c>
+      <c r="J85" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" t="s">
+        <v>138</v>
+      </c>
+      <c r="D86" t="s">
+        <v>158</v>
+      </c>
+      <c r="E86" t="s">
+        <v>227</v>
+      </c>
+      <c r="F86" t="s">
+        <v>310</v>
+      </c>
+      <c r="G86" t="s">
+        <v>321</v>
+      </c>
+      <c r="H86" t="s">
+        <v>384</v>
+      </c>
+      <c r="I86" t="s">
+        <v>434</v>
+      </c>
+      <c r="J86" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" t="s">
+        <v>138</v>
+      </c>
+      <c r="D87" t="s">
+        <v>158</v>
+      </c>
+      <c r="E87" t="s">
+        <v>227</v>
+      </c>
+      <c r="F87" t="s">
+        <v>277</v>
+      </c>
+      <c r="G87" t="s">
+        <v>321</v>
+      </c>
+      <c r="H87" t="s">
+        <v>385</v>
+      </c>
+      <c r="I87" t="s">
+        <v>434</v>
+      </c>
+      <c r="J87" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" t="s">
+        <v>150</v>
+      </c>
+      <c r="D88" t="s">
+        <v>158</v>
+      </c>
+      <c r="E88" t="s">
+        <v>228</v>
+      </c>
+      <c r="F88" t="s">
+        <v>270</v>
+      </c>
+      <c r="G88" t="s">
+        <v>321</v>
+      </c>
+      <c r="H88" t="s">
+        <v>386</v>
+      </c>
+      <c r="I88" t="s">
+        <v>417</v>
+      </c>
+      <c r="J88" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" t="s">
         <v>90</v>
       </c>
-      <c r="I21" t="s">
+      <c r="B89" t="s">
+        <v>106</v>
+      </c>
+      <c r="C89" t="s">
+        <v>138</v>
+      </c>
+      <c r="D89" t="s">
+        <v>158</v>
+      </c>
+      <c r="E89" t="s">
+        <v>229</v>
+      </c>
+      <c r="F89" t="s">
+        <v>311</v>
+      </c>
+      <c r="G89" t="s">
+        <v>321</v>
+      </c>
+      <c r="H89" t="s">
+        <v>338</v>
+      </c>
+      <c r="I89" t="s">
+        <v>435</v>
+      </c>
+      <c r="J89" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" t="s">
+        <v>117</v>
+      </c>
+      <c r="D90" t="s">
+        <v>158</v>
+      </c>
+      <c r="E90" t="s">
+        <v>230</v>
+      </c>
+      <c r="F90" t="s">
+        <v>312</v>
+      </c>
+      <c r="G90" t="s">
+        <v>321</v>
+      </c>
+      <c r="H90" t="s">
+        <v>351</v>
+      </c>
+      <c r="I90" t="s">
+        <v>436</v>
+      </c>
+      <c r="J90" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" t="s">
+        <v>151</v>
+      </c>
+      <c r="D91" t="s">
+        <v>158</v>
+      </c>
+      <c r="E91" t="s">
+        <v>231</v>
+      </c>
+      <c r="F91" t="s">
+        <v>313</v>
+      </c>
+      <c r="G91" t="s">
+        <v>321</v>
+      </c>
+      <c r="H91" t="s">
+        <v>348</v>
+      </c>
+      <c r="I91" t="s">
+        <v>437</v>
+      </c>
+      <c r="J91" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" t="s">
+        <v>106</v>
+      </c>
+      <c r="C92" t="s">
+        <v>152</v>
+      </c>
+      <c r="D92" t="s">
+        <v>158</v>
+      </c>
+      <c r="E92" t="s">
+        <v>232</v>
+      </c>
+      <c r="F92" t="s">
+        <v>314</v>
+      </c>
+      <c r="G92" t="s">
+        <v>321</v>
+      </c>
+      <c r="H92" t="s">
+        <v>387</v>
+      </c>
+      <c r="I92" t="s">
+        <v>438</v>
+      </c>
+      <c r="J92" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" t="s">
+        <v>152</v>
+      </c>
+      <c r="D93" t="s">
+        <v>158</v>
+      </c>
+      <c r="E93" t="s">
+        <v>233</v>
+      </c>
+      <c r="F93" t="s">
+        <v>315</v>
+      </c>
+      <c r="G93" t="s">
+        <v>321</v>
+      </c>
+      <c r="H93" t="s">
+        <v>351</v>
+      </c>
+      <c r="I93" t="s">
+        <v>438</v>
+      </c>
+      <c r="J93" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" t="s">
+        <v>153</v>
+      </c>
+      <c r="D94" t="s">
+        <v>158</v>
+      </c>
+      <c r="E94" t="s">
+        <v>234</v>
+      </c>
+      <c r="F94" t="s">
+        <v>316</v>
+      </c>
+      <c r="G94" t="s">
+        <v>321</v>
+      </c>
+      <c r="H94" t="s">
+        <v>388</v>
+      </c>
+      <c r="I94" t="s">
+        <v>438</v>
+      </c>
+      <c r="J94" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" t="s">
+        <v>106</v>
+      </c>
+      <c r="C95" t="s">
+        <v>154</v>
+      </c>
+      <c r="D95" t="s">
+        <v>158</v>
+      </c>
+      <c r="E95" t="s">
+        <v>235</v>
+      </c>
+      <c r="F95" t="s">
+        <v>303</v>
+      </c>
+      <c r="G95" t="s">
+        <v>321</v>
+      </c>
+      <c r="H95" t="s">
+        <v>389</v>
+      </c>
+      <c r="I95" t="s">
+        <v>438</v>
+      </c>
+      <c r="J95" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96" t="s">
+        <v>155</v>
+      </c>
+      <c r="D96" t="s">
+        <v>158</v>
+      </c>
+      <c r="E96" t="s">
+        <v>236</v>
+      </c>
+      <c r="F96" t="s">
+        <v>317</v>
+      </c>
+      <c r="G96" t="s">
+        <v>321</v>
+      </c>
+      <c r="H96" t="s">
+        <v>390</v>
+      </c>
+      <c r="I96" t="s">
+        <v>438</v>
+      </c>
+      <c r="J96" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" t="s">
+        <v>106</v>
+      </c>
+      <c r="C97" t="s">
+        <v>156</v>
+      </c>
+      <c r="D97" t="s">
+        <v>158</v>
+      </c>
+      <c r="E97" t="s">
+        <v>237</v>
+      </c>
+      <c r="F97" t="s">
+        <v>301</v>
+      </c>
+      <c r="G97" t="s">
+        <v>321</v>
+      </c>
+      <c r="H97" t="s">
+        <v>391</v>
+      </c>
+      <c r="I97" t="s">
+        <v>438</v>
+      </c>
+      <c r="J97" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" t="s">
+        <v>117</v>
+      </c>
+      <c r="D98" t="s">
+        <v>158</v>
+      </c>
+      <c r="E98" t="s">
+        <v>238</v>
+      </c>
+      <c r="F98" t="s">
+        <v>266</v>
+      </c>
+      <c r="G98" t="s">
+        <v>321</v>
+      </c>
+      <c r="H98" t="s">
+        <v>334</v>
+      </c>
+      <c r="I98" t="s">
+        <v>404</v>
+      </c>
+      <c r="J98" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" t="s">
+        <v>106</v>
+      </c>
+      <c r="C99" t="s">
+        <v>157</v>
+      </c>
+      <c r="D99" t="s">
+        <v>158</v>
+      </c>
+      <c r="E99" t="s">
+        <v>239</v>
+      </c>
+      <c r="F99" t="s">
+        <v>318</v>
+      </c>
+      <c r="G99" t="s">
+        <v>321</v>
+      </c>
+      <c r="H99" t="s">
+        <v>392</v>
+      </c>
+      <c r="I99" t="s">
+        <v>408</v>
+      </c>
+      <c r="J99" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" t="s">
+        <v>106</v>
+      </c>
+      <c r="C100" t="s">
+        <v>115</v>
+      </c>
+      <c r="D100" t="s">
+        <v>158</v>
+      </c>
+      <c r="E100" t="s">
+        <v>240</v>
+      </c>
+      <c r="F100" t="s">
+        <v>319</v>
+      </c>
+      <c r="G100" t="s">
+        <v>321</v>
+      </c>
+      <c r="H100" t="s">
+        <v>393</v>
+      </c>
+      <c r="I100" t="s">
+        <v>395</v>
+      </c>
+      <c r="J100" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" t="s">
         <v>102</v>
       </c>
-      <c r="J21" t="s">
-        <v>108</v>
+      <c r="B101" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" t="s">
+        <v>138</v>
+      </c>
+      <c r="D101" t="s">
+        <v>158</v>
+      </c>
+      <c r="E101" t="s">
+        <v>241</v>
+      </c>
+      <c r="F101" t="s">
+        <v>320</v>
+      </c>
+      <c r="G101" t="s">
+        <v>321</v>
+      </c>
+      <c r="H101" t="s">
+        <v>394</v>
+      </c>
+      <c r="I101" t="s">
+        <v>439</v>
+      </c>
+      <c r="J101" t="s">
+        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>